<commit_message>
work done friday 26 may
</commit_message>
<xml_diff>
--- a/Matlab_Stuff/time taken.xlsx
+++ b/Matlab_Stuff/time taken.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Documents\study Stevens\Boundary Layer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Documents\BoundaryLayer\Matlab_Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>L=4, h1=1.2, h2=0.8</t>
   </si>
@@ -42,19 +43,37 @@
   </si>
   <si>
     <t>doesn't work</t>
+  </si>
+  <si>
+    <t>x [m]</t>
+  </si>
+  <si>
+    <t>τ [N/m^2] - example</t>
+  </si>
+  <si>
+    <t>τ [N/m^2] - program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -73,12 +92,133 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -461,4 +601,68 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6.07</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.92</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10">
+        <v>6.27</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.982</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.627</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>